<commit_message>
Create Credit Memo, Create Accept Payment, Create Show Address
</commit_message>
<xml_diff>
--- a/InputData/Customers_details.xlsx
+++ b/InputData/Customers_details.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2440" windowWidth="13060" windowHeight="6060"/>
+    <workbookView xWindow="0" yWindow="2440" windowWidth="14690" windowHeight="6060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="70">
   <si>
     <t>Email</t>
   </si>
@@ -127,9 +127,6 @@
     <t>PAN</t>
   </si>
   <si>
-    <t>Quick 2019/11/22 19:03:47</t>
-  </si>
-  <si>
     <t>Project Name</t>
   </si>
   <si>
@@ -154,172 +151,82 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>Quick 2019/11/23 18:13:15</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/23 18:14:04</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/23 19:05:27</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/23 19:06:17</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/23 19:19:56</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/23 19:20:47</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/23 21:36:02</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/23 21:42:20</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/23 22:08:13</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/23 22:11:40</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/23 22:12:25</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/23 22:28:02</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/23 22:28:48</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/23 23:17:57</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/23 23:18:46</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/23 23:29:39</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/23 23:39:40</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/23 23:45:01</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/23 23:52:58</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/24 00:17:51</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/24 00:21:58</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/24 00:22:54</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/24 00:27:21</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/24 00:28:17</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/24 00:32:09</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/24 00:33:04</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/24 19:37:24</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/24 19:38:13</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/24 19:45:20</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/24 19:46:09</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/24 23:54:51</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/24 23:55:53</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 00:05:10</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 00:06:24</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 00:13:46</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 00:16:39</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 00:21:42</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 00:24:18</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 00:30:44</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 00:37:30</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 00:43:09</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 00:47:12</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 00:53:05</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 00:54:03</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 01:03:13</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 10:10:44</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 10:15:41</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 10:19:44</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 10:20:36</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 10:22:21</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 10:23:15</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 10:34:25</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 10:38:33</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 10:39:25</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 10:45:16</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 10:46:10</t>
+    <t>Invoice Number</t>
+  </si>
+  <si>
+    <t>Payment mode</t>
+  </si>
+  <si>
+    <t>Payment Mode Details</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>Online Bank</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Local</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Address Name</t>
+  </si>
+  <si>
+    <t>INV-516-261119-38</t>
+  </si>
+  <si>
+    <t>Quick 2019/11/26 11:19:23</t>
+  </si>
+  <si>
+    <t>Quick 2019/11/26 12:51:52</t>
+  </si>
+  <si>
+    <t>Quick 2019/11/26 12:52:45</t>
+  </si>
+  <si>
+    <t>INV-520-261119-41</t>
+  </si>
+  <si>
+    <t>300.00</t>
+  </si>
+  <si>
+    <t>Quick 2019/11/26 13:44:56</t>
+  </si>
+  <si>
+    <t>Quick 2019/11/26 13:45:53</t>
+  </si>
+  <si>
+    <t>INV-521-261119-42</t>
+  </si>
+  <si>
+    <t>Quick 2019/11/26 13:59:14</t>
+  </si>
+  <si>
+    <t>Quick 2019/11/26 14:00:10</t>
+  </si>
+  <si>
+    <t>INV-522-261119-43</t>
+  </si>
+  <si>
+    <t>Quick 2019/11/26 14:27:32</t>
+  </si>
+  <si>
+    <t>Quick 2019/11/26 14:28:24</t>
+  </si>
+  <si>
+    <t>INV-523-261119-44</t>
+  </si>
+  <si>
+    <t>300</t>
   </si>
 </sst>
 </file>
@@ -671,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA2"/>
+  <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="Y6" sqref="Y6"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AE2" sqref="AE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -688,12 +595,10 @@
     <col min="8" max="8" customWidth="true" style="1" width="9.90625" collapsed="true"/>
     <col min="9" max="16" style="1" width="8.7265625" collapsed="true"/>
     <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="10.81640625" collapsed="true"/>
-    <col min="18" max="25" style="1" width="8.7265625" collapsed="true"/>
-    <col min="26" max="26" style="1" width="8.7265625" collapsed="true"/>
-    <col min="27" max="16384" style="1" width="8.7265625" collapsed="true"/>
+    <col min="18" max="16384" style="1" width="8.7265625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="43.5">
+    <row r="1" spans="1:33" ht="43.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -758,25 +663,43 @@
         <v>35</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="W1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="Z1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AA1" s="1" t="s">
-        <v>43</v>
+      <c r="AC1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="43.5">
+    <row r="2" spans="1:33" ht="43.5">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -784,7 +707,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>100</v>
+        <v>67</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>15</v>
@@ -841,7 +764,7 @@
         <v>1234567</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="W2" s="1">
         <v>1234567</v>
@@ -850,13 +773,31 @@
         <v>1234567</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Z2" s="1">
         <v>3</v>
       </c>
       <c r="AA2" s="1">
         <v>100</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>199</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create Expense Test script added
</commit_message>
<xml_diff>
--- a/InputData/Customers_details.xlsx
+++ b/InputData/Customers_details.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>Email</t>
   </si>
@@ -160,15 +160,9 @@
     <t>Payment Mode Details</t>
   </si>
   <si>
-    <t>Cash</t>
-  </si>
-  <si>
     <t>Online Bank</t>
   </si>
   <si>
-    <t>Amount</t>
-  </si>
-  <si>
     <t>Local</t>
   </si>
   <si>
@@ -181,52 +175,58 @@
     <t>Address Name</t>
   </si>
   <si>
-    <t>INV-516-261119-38</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/26 11:19:23</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/26 12:51:52</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/26 12:52:45</t>
-  </si>
-  <si>
-    <t>INV-520-261119-41</t>
-  </si>
-  <si>
     <t>300.00</t>
   </si>
   <si>
-    <t>Quick 2019/11/26 13:44:56</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/26 13:45:53</t>
-  </si>
-  <si>
-    <t>INV-521-261119-42</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/26 13:59:14</t>
-  </si>
-  <si>
     <t>Quick 2019/11/26 14:00:10</t>
   </si>
   <si>
     <t>INV-522-261119-43</t>
   </si>
   <si>
-    <t>Quick 2019/11/26 14:27:32</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/26 14:28:24</t>
-  </si>
-  <si>
-    <t>INV-523-261119-44</t>
+    <t>Expense Type</t>
+  </si>
+  <si>
+    <t>Expense Amount</t>
+  </si>
+  <si>
+    <t>Payment Amount</t>
+  </si>
+  <si>
+    <t>Shipping Expense</t>
+  </si>
+  <si>
+    <t>Expense Number</t>
+  </si>
+  <si>
+    <t>EXP-524-261119-3</t>
+  </si>
+  <si>
+    <t>EXP-524-261119-4</t>
+  </si>
+  <si>
+    <t>EXP-524-261119-5</t>
+  </si>
+  <si>
+    <t>EXP-524-261119-6</t>
+  </si>
+  <si>
+    <t>EXP-524-261119-7</t>
+  </si>
+  <si>
+    <t>Quick 2019/11/26 18:57:15</t>
+  </si>
+  <si>
+    <t>Quick 2019/11/26 18:58:19</t>
+  </si>
+  <si>
+    <t>INV-526-261119-45</t>
   </si>
   <si>
     <t>300</t>
+  </si>
+  <si>
+    <t>EXP-526-261119-8</t>
   </si>
 </sst>
 </file>
@@ -578,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AG2"/>
+  <dimension ref="A1:AJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AE2" sqref="AE2"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AE8" sqref="AE8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -598,7 +598,7 @@
     <col min="18" max="16384" style="1" width="8.7265625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="43.5">
+    <row r="1" spans="1:36" ht="43.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -690,16 +690,25 @@
         <v>46</v>
       </c>
       <c r="AE1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AF1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>51</v>
+      <c r="AH1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="43.5">
+    <row r="2" spans="1:36" ht="43.5">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -707,7 +716,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>15</v>
@@ -782,22 +791,28 @@
         <v>100</v>
       </c>
       <c r="AB2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC2" t="s">
         <v>68</v>
       </c>
-      <c r="AC2" t="s">
-        <v>69</v>
-      </c>
       <c r="AD2" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AE2" s="1">
         <v>199</v>
       </c>
       <c r="AF2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AG2" s="1" t="s">
-        <v>52</v>
+      <c r="AH2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI2" s="1">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed DeleteCustomer, CreateSO, LogActivity, LogCommunication, ActionPerform by Nitin.
</commit_message>
<xml_diff>
--- a/InputData/Customers_details.xlsx
+++ b/InputData/Customers_details.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2440" windowWidth="13060" windowHeight="6060"/>
+    <workbookView xWindow="0" yWindow="2440" windowWidth="14690" windowHeight="6060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>Email</t>
   </si>
@@ -127,9 +127,6 @@
     <t>PAN</t>
   </si>
   <si>
-    <t>Quick 2019/11/22 19:03:47</t>
-  </si>
-  <si>
     <t>Project Name</t>
   </si>
   <si>
@@ -154,172 +151,82 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>Quick 2019/11/23 18:13:15</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/23 18:14:04</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/23 19:05:27</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/23 19:06:17</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/23 19:19:56</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/23 19:20:47</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/23 21:36:02</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/23 21:42:20</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/23 22:08:13</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/23 22:11:40</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/23 22:12:25</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/23 22:28:02</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/23 22:28:48</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/23 23:17:57</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/23 23:18:46</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/23 23:29:39</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/23 23:39:40</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/23 23:45:01</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/23 23:52:58</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/24 00:17:51</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/24 00:21:58</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/24 00:22:54</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/24 00:27:21</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/24 00:28:17</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/24 00:32:09</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/24 00:33:04</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/24 19:37:24</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/24 19:38:13</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/24 19:45:20</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/24 19:46:09</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/24 23:54:51</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/24 23:55:53</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 00:05:10</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 00:06:24</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 00:13:46</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 00:16:39</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 00:21:42</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 00:24:18</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 00:30:44</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 00:37:30</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 00:43:09</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 00:47:12</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 00:53:05</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 00:54:03</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 01:03:13</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 10:10:44</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 10:15:41</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 10:19:44</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 10:20:36</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 10:22:21</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 10:23:15</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 10:34:25</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 10:38:33</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 10:39:25</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 10:45:16</t>
-  </si>
-  <si>
-    <t>Quick 2019/11/25 10:46:10</t>
+    <t>Invoice Number</t>
+  </si>
+  <si>
+    <t>Payment mode</t>
+  </si>
+  <si>
+    <t>Payment Mode Details</t>
+  </si>
+  <si>
+    <t>Online Bank</t>
+  </si>
+  <si>
+    <t>Local</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Address Name</t>
+  </si>
+  <si>
+    <t>300.00</t>
+  </si>
+  <si>
+    <t>Quick 2019/11/26 14:00:10</t>
+  </si>
+  <si>
+    <t>INV-522-261119-43</t>
+  </si>
+  <si>
+    <t>Expense Type</t>
+  </si>
+  <si>
+    <t>Expense Amount</t>
+  </si>
+  <si>
+    <t>Payment Amount</t>
+  </si>
+  <si>
+    <t>Shipping Expense</t>
+  </si>
+  <si>
+    <t>Expense Number</t>
+  </si>
+  <si>
+    <t>EXP-524-261119-3</t>
+  </si>
+  <si>
+    <t>EXP-524-261119-4</t>
+  </si>
+  <si>
+    <t>EXP-524-261119-5</t>
+  </si>
+  <si>
+    <t>EXP-524-261119-6</t>
+  </si>
+  <si>
+    <t>EXP-524-261119-7</t>
+  </si>
+  <si>
+    <t>Quick 2019/11/26 18:57:15</t>
+  </si>
+  <si>
+    <t>Quick 2019/11/26 18:58:19</t>
+  </si>
+  <si>
+    <t>INV-526-261119-45</t>
+  </si>
+  <si>
+    <t>300</t>
+  </si>
+  <si>
+    <t>EXP-526-261119-8</t>
   </si>
 </sst>
 </file>
@@ -671,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA2"/>
+  <dimension ref="A1:AJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="Y6" sqref="Y6"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AE8" sqref="AE8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -688,12 +595,10 @@
     <col min="8" max="8" customWidth="true" style="1" width="9.90625" collapsed="true"/>
     <col min="9" max="16" style="1" width="8.7265625" collapsed="true"/>
     <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="10.81640625" collapsed="true"/>
-    <col min="18" max="25" style="1" width="8.7265625" collapsed="true"/>
-    <col min="26" max="26" style="1" width="8.7265625" collapsed="true"/>
-    <col min="27" max="16384" style="1" width="8.7265625" collapsed="true"/>
+    <col min="18" max="16384" style="1" width="8.7265625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="43.5">
+    <row r="1" spans="1:36" ht="43.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -758,25 +663,52 @@
         <v>35</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="W1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="Z1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AA1" s="1" t="s">
-        <v>43</v>
+      <c r="AC1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="43.5">
+    <row r="2" spans="1:36" ht="43.5">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -784,7 +716,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>100</v>
+        <v>66</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>15</v>
@@ -841,7 +773,7 @@
         <v>1234567</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="W2" s="1">
         <v>1234567</v>
@@ -850,12 +782,36 @@
         <v>1234567</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Z2" s="1">
         <v>3</v>
       </c>
       <c r="AA2" s="1">
+        <v>100</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>199</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI2" s="1">
         <v>100</v>
       </c>
     </row>

</xml_diff>